<commit_message>
updated scripts with latest command listing
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/execution-meta/artifact/data/execution-meta.data.xlsx
+++ b/examples/execution-meta/artifact/data/execution-meta.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10203"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10708"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/examples/execution-meta/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5444E3A2-08A9-6A46-9CB8-DE16CCD2088D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5647D572-A89F-AE47-B71A-CC0E8BE422E2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34140" yWindow="440" windowWidth="17060" windowHeight="31560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34140" yWindow="460" windowWidth="17060" windowHeight="31540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -582,7 +582,7 @@
   <dimension ref="A1:AAA200"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>

</xml_diff>